<commit_message>
agregados parte de la entrega
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TEIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B6E266-1DE9-49E7-86F5-31778F20015D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413C9DD2-B2EA-495B-A21A-B938A7608CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F6CAEB3-32EA-4598-8AEF-777457DAD3A7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Nombre funcionalidad</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>BorrarComentario</t>
+  </si>
+  <si>
+    <t>AgregarDireccion</t>
+  </si>
+  <si>
+    <t>UserController</t>
+  </si>
+  <si>
+    <t>ObtenerDireccion</t>
+  </si>
+  <si>
+    <t>ItemController</t>
+  </si>
+  <si>
+    <t>VerCompras</t>
+  </si>
+  <si>
+    <t>Comprar</t>
+  </si>
+  <si>
+    <t>BuyOrderController</t>
+  </si>
+  <si>
+    <t>AgregarACarrito</t>
+  </si>
+  <si>
+    <t>CartController</t>
+  </si>
+  <si>
+    <t>verVentas</t>
   </si>
 </sst>
 </file>
@@ -504,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBB1EB1-8D5E-434A-B7AB-39A412C4458F}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,6 +668,72 @@
         <v>52</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>